<commit_message>
First individual 5 hrs finished
I am stuck on a tiny problem which is the problem of NameSpace. Trying to work out, but failed. I would ask Nare in the class
</commit_message>
<xml_diff>
--- a/week1HelloWorldMVC/timesheet_Wei_Liu_317932.xlsx
+++ b/week1HelloWorldMVC/timesheet_Wei_Liu_317932.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>WEE</t>
   </si>
@@ -83,6 +83,25 @@
   </si>
   <si>
     <t xml:space="preserve">Talking about the individual progress and try to put everyone on the same paper. Sharing the problems that each person is stuck on. </t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>Being familiar with what is the MVC. Including how they will process, who they will work.</t>
+  </si>
+  <si>
+    <t>23/7/2020</t>
+  </si>
+  <si>
+    <t>tutorial Part 1 +Part 2. Setting up VS 2009 and installing IDK, examine the function of a controller. Coding some others to change exist codes</t>
+  </si>
+  <si>
+    <t>Tutorial Part 3+ Part 4, understand the relationship between View, Model and Controller. The main idea is ViewData dictionary was used to pass data from the controller to a view.</t>
+  </si>
+  <si>
+    <t>Tutorial Part 5, I was stuck on a problem which is a namespcae could not be found. It spend me for almost 1.5 hours to work on it, but I did not work it out.
+Meanwhile, I understood how to develop a database in C# and operate DB</t>
   </si>
 </sst>
 </file>
@@ -125,7 +144,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -441,16 +460,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="14.69921875" customWidth="1"/>
-    <col min="3" max="3" width="105.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="134.796875" customWidth="1"/>
     <col min="4" max="4" width="19.8984375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -497,7 +516,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -509,6 +528,66 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
all individual 10 hrs done
</commit_message>
<xml_diff>
--- a/week1HelloWorldMVC/timesheet_Wei_Liu_317932.xlsx
+++ b/week1HelloWorldMVC/timesheet_Wei_Liu_317932.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>WEE</t>
   </si>
@@ -108,6 +108,20 @@
   </si>
   <si>
     <t>29/7/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tutorial Part 7 searching, there are two ways to create search, one is to modify URL, another is to add table into view. But the later way is the best to help users operate.
+Understood the way of adding search function.
+</t>
+  </si>
+  <si>
+    <t>Tutorial Part 8, studying how to add a new filed, when there will be a new field, all others will be updated based on new version. However, because of a tiny problem, my app can not process well.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tutorial Part 9 +10 , how to create validation rules that would be forced any time when users create or edit a movie. Meanwhile, explictly understood the details of fucntions of detail and delete. </t>
+  </si>
+  <si>
+    <t>Review the whole tutorial of MVC, tested and played some of them parts, trying to understand how to build my own website.</t>
   </si>
 </sst>
 </file>
@@ -466,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -605,6 +619,62 @@
         <v>21</v>
       </c>
     </row>
+    <row r="10" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2 hrs team meeting
</commit_message>
<xml_diff>
--- a/week1HelloWorldMVC/timesheet_Wei_Liu_317932.xlsx
+++ b/week1HelloWorldMVC/timesheet_Wei_Liu_317932.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
   <si>
     <t>WEE</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>Review the whole tutorial of MVC, tested and played some of them parts, trying to understand how to build my own website.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed some problems related to database and namespace. Sharing some ideas </t>
   </si>
 </sst>
 </file>
@@ -480,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -549,32 +552,29 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -585,24 +585,24 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>19</v>
+      <c r="C8" t="s">
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -613,24 +613,24 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -641,21 +641,21 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
         <v>21</v>
@@ -669,9 +669,37 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
         <v>25</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D15" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>